<commit_message>
added option to remove parantheses from title for songs
</commit_message>
<xml_diff>
--- a/data/all songs with not found uri.xlsx
+++ b/data/all songs with not found uri.xlsx
@@ -34567,7 +34567,7 @@
       </c>
       <c r="F1140" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>spotify:track:3kqXhOP3kzCuqT5Xj689Dr</t>
         </is>
       </c>
     </row>
@@ -35035,7 +35035,7 @@
       </c>
       <c r="F1156" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>spotify:track:4WiFBRzY34rxXOVDc679Oh</t>
         </is>
       </c>
     </row>
@@ -35063,7 +35063,7 @@
       </c>
       <c r="F1157" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>spotify:track:1AdXchAT6hBUm5d6y4nKjI</t>
         </is>
       </c>
     </row>
@@ -35091,7 +35091,7 @@
       </c>
       <c r="F1158" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>spotify:track:3JKgcAa7r07ocVWcV8bS0H</t>
         </is>
       </c>
     </row>
@@ -35149,7 +35149,7 @@
       </c>
       <c r="F1160" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>spotify:track:3KFKxDnP39CnCZukcLFzSO</t>
         </is>
       </c>
     </row>
@@ -35237,7 +35237,7 @@
       </c>
       <c r="F1163" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>spotify:track:3y3NwQPQAjKCunRz2eKggA</t>
         </is>
       </c>
     </row>
@@ -35265,7 +35265,7 @@
       </c>
       <c r="F1164" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>spotify:track:2iW6Hb6kfrz2K7EhPibFiq</t>
         </is>
       </c>
     </row>
@@ -35293,7 +35293,7 @@
       </c>
       <c r="F1165" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>spotify:track:2toC43RDMMNjm1wDP65EJF</t>
         </is>
       </c>
     </row>
@@ -35351,7 +35351,7 @@
       </c>
       <c r="F1167" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>spotify:track:16iEQmgEaqLnwY545oowAB</t>
         </is>
       </c>
     </row>
@@ -35409,7 +35409,7 @@
       </c>
       <c r="F1169" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>spotify:track:1BaJfy4b4vdwQ6NLbcGPfF</t>
         </is>
       </c>
     </row>
@@ -35587,7 +35587,7 @@
       </c>
       <c r="F1175" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>spotify:track:2U9a9vMEGjEnQ4YI5HBwBB</t>
         </is>
       </c>
     </row>
@@ -35615,7 +35615,7 @@
       </c>
       <c r="F1176" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>spotify:track:2fRoKHW3lzNUKIUTade8nL</t>
         </is>
       </c>
     </row>
@@ -35643,7 +35643,7 @@
       </c>
       <c r="F1177" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>spotify:track:0sKEilrw1GrBlG6qsTCrP4</t>
         </is>
       </c>
     </row>
@@ -35671,7 +35671,7 @@
       </c>
       <c r="F1178" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>spotify:track:1Ug5wxoHthwxctyWTUMGta</t>
         </is>
       </c>
     </row>
@@ -35699,7 +35699,7 @@
       </c>
       <c r="F1179" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>spotify:track:5QLHGv0DfpeXLNFo7SFEy1</t>
         </is>
       </c>
     </row>
@@ -35727,7 +35727,7 @@
       </c>
       <c r="F1180" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>spotify:track:1p1b9LdLJ0REuFJX9mYtFX</t>
         </is>
       </c>
     </row>
@@ -35755,7 +35755,7 @@
       </c>
       <c r="F1181" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>spotify:track:0oFZrjptKqIOj6yw5zjuDx</t>
         </is>
       </c>
     </row>
@@ -35783,7 +35783,7 @@
       </c>
       <c r="F1182" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>spotify:track:53H2tt0Km67kNl37dj8y5b</t>
         </is>
       </c>
     </row>
@@ -35839,7 +35839,7 @@
       </c>
       <c r="F1184" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>spotify:track:1mIzI74ftRcKIK1Df0JlGQ</t>
         </is>
       </c>
     </row>
@@ -35867,7 +35867,7 @@
       </c>
       <c r="F1185" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>spotify:track:1e3GEwsaXtBNtPfooQimDn</t>
         </is>
       </c>
     </row>
@@ -35895,7 +35895,7 @@
       </c>
       <c r="F1186" t="inlineStr">
         <is>
-          <t>NOT FOUND</t>
+          <t>spotify:track:5DT26VHeeY5lDUP3vPZr77</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updating flow and variable names
</commit_message>
<xml_diff>
--- a/data/all songs with not found uri.xlsx
+++ b/data/all songs with not found uri.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="firework" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="yew" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -47,9 +47,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -433,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,36 +472,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Pursuit of Happiness (feat. MGMT &amp; Ratatat) [Extended Steve Aoki Remix]</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>0.2597222222222222</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Kid Cudi</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Pursuit of Happiness (feat. MGMT &amp; Ratatat) [Extended Steve Aoki Remix] - Single</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Hip-Hop/Rap</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>NOT FOUND</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>